<commit_message>
update with new review RTM and SRS
</commit_message>
<xml_diff>
--- a/PMP/Review sheet.xlsx
+++ b/PMP/Review sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hamada\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA\workshop\review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC89382-6508-4743-B9DB-AA1E1DE40B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A83D5DA-22EB-4CA2-8E6A-8BAD69C5F0D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F7B8BED2-8B5E-4E93-BD0C-B9ADFADDDD77}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
   <si>
     <t>the document</t>
   </si>
@@ -184,6 +184,23 @@
   </si>
   <si>
     <t xml:space="preserve"> I suggest to  add status colum</t>
+  </si>
+  <si>
+    <t>SRS_02</t>
+  </si>
+  <si>
+    <t>Nourhan Ali,Mohamed Ibrahim
+,Manar Ali ,Aalaa Adel and Al-Shimaa
+Shehata</t>
+  </si>
+  <si>
+    <t>__</t>
+  </si>
+  <si>
+    <t>RTM_01</t>
+  </si>
+  <si>
+    <t>Requirment Tracability Matrix</t>
   </si>
 </sst>
 </file>
@@ -263,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -272,26 +289,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -311,9 +337,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -351,7 +377,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -457,7 +483,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -599,7 +625,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -607,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD6593F-9E28-4ADE-BC92-8F83CD20BE79}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,26 +652,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -680,184 +706,236 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="21" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="21" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="11">
+        <v>45508</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="12">
+        <v>45508</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>